<commit_message>
running notes from 10-16
</commit_message>
<xml_diff>
--- a/running-notes.xlsx
+++ b/running-notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DevOps-Process" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
   <si>
     <t>Continuous Integration</t>
   </si>
@@ -302,12 +302,102 @@
   <si>
     <t>git config —global user.email “&lt;email-id&gt;”</t>
   </si>
+  <si>
+    <t>Folder Structure</t>
+  </si>
+  <si>
+    <t>&lt;app-name&gt;/src/main/java/&lt;company/project-name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;app-name&gt;/src/test/java/&lt;company/project-name&gt;</t>
+  </si>
+  <si>
+    <t>POM.xml</t>
+  </si>
+  <si>
+    <t>Project Object Model</t>
+  </si>
+  <si>
+    <t>GAV</t>
+  </si>
+  <si>
+    <t>Group-Id</t>
+  </si>
+  <si>
+    <t>Artifact-Id</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Repositories</t>
+  </si>
+  <si>
+    <t>Artifact repo -&gt; Where we store all of our artifacts(Deploy phase)</t>
+  </si>
+  <si>
+    <t>m2 repo -&gt; Local repository from where you run any mvn commands</t>
+  </si>
+  <si>
+    <t>Central repo -&gt; Maven repo</t>
+  </si>
+  <si>
+    <t>.m2 repo</t>
+  </si>
+  <si>
+    <t>We will have all the plug-ins, libraries, artifacts stored</t>
+  </si>
+  <si>
+    <t>settings.xml-&gt; where we will define our uname/passwrd, over-write settings to no to go to Maven’s central repo</t>
+  </si>
+  <si>
+    <t>Plugins</t>
+  </si>
+  <si>
+    <t>First you run any maven in local, it will take long time to execute.</t>
+  </si>
+  <si>
+    <t>Dependency Mngmnt</t>
+  </si>
+  <si>
+    <t>To compile any java code, we need libraries. Libraries will be defined in dependency mngmnt</t>
+  </si>
+  <si>
+    <t>Release types</t>
+  </si>
+  <si>
+    <t>SNAPSHOT -&gt; Project version(1.0-SNAPSHOT)</t>
+  </si>
+  <si>
+    <t>Release -&gt; (1.0) it is ready to roll-out to PROD</t>
+  </si>
+  <si>
+    <t>Release process</t>
+  </si>
+  <si>
+    <t>1.0-SNAPSHOT -&gt; 1.0 -&gt; [1.1/2.0]-SNAPSHOT</t>
+  </si>
+  <si>
+    <t>&lt;groupId&gt;com.orrbasystems&lt;/groupId&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;artifactId&gt;october&lt;/artifactId&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;packaging&gt;jar&lt;/packaging&gt;</t>
+  </si>
+  <si>
+    <t>  &lt;version&gt;1.0-SNAPSHOT&lt;/version&gt;</t>
+  </si>
+  <si>
+    <t>com/orrbasystems/october/1.0-SNAPSHOT/october-1.0-SNAPSHOT.jar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -353,6 +443,11 @@
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -374,31 +469,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,16 +827,16 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -746,25 +844,25 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="F6" s="6"/>
+      <c r="D6" s="15"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="54" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="9" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
@@ -818,34 +916,34 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -971,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E43"/>
+  <dimension ref="A3:E75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C25"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,7 +1080,7 @@
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="82.6640625" customWidth="1"/>
+    <col min="4" max="4" width="118.33203125" customWidth="1"/>
     <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -994,7 +1092,7 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="1"/>
@@ -1004,35 +1102,35 @@
     </row>
     <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="1"/>
@@ -1048,11 +1146,11 @@
     </row>
     <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="1"/>
@@ -1061,7 +1159,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="1"/>
@@ -1081,11 +1179,11 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="40" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D13" s="1"/>
@@ -1095,7 +1193,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E14" s="1"/>
@@ -1104,7 +1202,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="1"/>
@@ -1113,7 +1211,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="1"/>
@@ -1122,7 +1220,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E17" s="1"/>
@@ -1131,7 +1229,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="8" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="1"/>
@@ -1147,7 +1245,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="1"/>
@@ -1160,40 +1258,40 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="11" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="11" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="11" t="s">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="11" t="s">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
@@ -1210,7 +1308,7 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="1"/>
@@ -1221,37 +1319,37 @@
     <row r="29" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="13" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="13"/>
-      <c r="E31" s="5"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="18"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="11" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
@@ -1261,66 +1359,66 @@
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="11" t="s">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="15"/>
     </row>
     <row r="35" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="11" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="5"/>
+      <c r="E35" s="15"/>
     </row>
     <row r="36" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="11" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="5"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="11" t="s">
+      <c r="A37" s="17"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="39" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="11" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="5"/>
+      <c r="E39" s="15"/>
     </row>
     <row r="40" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="11" t="s">
+      <c r="A40" s="17"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="15"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
@@ -1336,15 +1434,246 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="B43" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="E43" s="1"/>
     </row>
+    <row r="44" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B44" s="18"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B46" s="5"/>
+      <c r="C46" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B48" s="15"/>
+      <c r="C48" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B49" s="15"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B50" s="15"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+    </row>
+    <row r="52" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B52" s="15"/>
+      <c r="C52" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B53" s="15"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B54" s="15"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B56" s="15"/>
+      <c r="C56" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B57" s="15"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B59" s="5"/>
+      <c r="C59" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B61" s="5"/>
+      <c r="C61" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B63" s="15"/>
+      <c r="C63" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B64" s="15"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B68" s="5"/>
+      <c r="C68" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="2:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="B70" s="15"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+    </row>
+    <row r="75" spans="2:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="24">
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C70:C75"/>
+    <mergeCell ref="B70:B75"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B56:B57"/>
     <mergeCell ref="E22:E25"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="B22:B25"/>
@@ -1366,7 +1695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1384,22 +1713,22 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -1410,22 +1739,22 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -1447,13 +1776,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="11" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1469,7 +1798,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="16">
+      <c r="B12" s="12">
         <v>43783</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1479,7 +1808,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="16">
+      <c r="B13" s="12">
         <v>43760</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1489,7 +1818,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="16">
+      <c r="B14" s="12">
         <v>43740</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1515,13 +1844,13 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="11" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C18" s="1"/>
@@ -1538,7 +1867,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="16">
+      <c r="B20" s="12">
         <v>43783</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1548,13 +1877,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="16">
+      <c r="B21" s="12">
         <v>43740</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="12">
         <v>43733</v>
       </c>
     </row>
@@ -1584,7 +1913,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="11" t="s">
         <v>73</v>
       </c>
       <c r="C25" s="1"/>
@@ -1601,7 +1930,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="16">
+      <c r="B27" s="12">
         <v>43740</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -1611,7 +1940,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <v>43731</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1633,7 +1962,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="16">
+      <c r="D30" s="12">
         <v>43729</v>
       </c>
     </row>
@@ -1659,7 +1988,7 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="11" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1693,7 +2022,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="11" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1719,7 +2048,7 @@
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="11" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating Oct 18th notes
</commit_message>
<xml_diff>
--- a/running-notes.xlsx
+++ b/running-notes.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="133">
   <si>
     <t>Continuous Integration</t>
   </si>
@@ -391,6 +391,66 @@
   </si>
   <si>
     <t>com/orrbasystems/october/1.0-SNAPSHOT/october-1.0-SNAPSHOT.jar</t>
+  </si>
+  <si>
+    <t>&lt;xml&gt; version and opening of project</t>
+  </si>
+  <si>
+    <t>packaging —&gt; jar/war/tar</t>
+  </si>
+  <si>
+    <t>dependencies —&gt; we define all our project dependencies</t>
+  </si>
+  <si>
+    <t>modules —&gt; To define all child components.</t>
+  </si>
+  <si>
+    <t>dependencyManagement</t>
+  </si>
+  <si>
+    <t>scm —&gt; we define our SCM URL</t>
+  </si>
+  <si>
+    <t>repositories —&gt; artifact Repository URL</t>
+  </si>
+  <si>
+    <t>pluginRepositories —&gt; Apache Maven’s Repo URL</t>
+  </si>
+  <si>
+    <t>distributionManagement —&gt; Artifact repository URL and will be used in “mvn deploy” phase</t>
+  </si>
+  <si>
+    <t>profiles —&gt; based on project/user/…</t>
+  </si>
+  <si>
+    <t>Parent/Child Module</t>
+  </si>
+  <si>
+    <t>pom.xml -&gt; parent POM</t>
+  </si>
+  <si>
+    <t>Wk1/pom.xml</t>
+  </si>
+  <si>
+    <t>Wk2/pom.xml</t>
+  </si>
+  <si>
+    <t>Wk3/pom.xml</t>
+  </si>
+  <si>
+    <t>Wk4/pom.xml</t>
+  </si>
+  <si>
+    <t>Release life cycle</t>
+  </si>
+  <si>
+    <t>Prepare —&gt; mvn release:prepare</t>
+  </si>
+  <si>
+    <t>Perform —&gt; mvn release:perform ( 1.0-SNPASHOT -&gt; 1.0, 1.1/2.0-SNAPSHOT)</t>
+  </si>
+  <si>
+    <t>Rollback —&gt; mvn release:rollback</t>
   </si>
 </sst>
 </file>
@@ -469,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -487,16 +547,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,16 +889,16 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -844,25 +906,25 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="F6" s="14"/>
+      <c r="D6" s="18"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="54" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
@@ -916,34 +978,34 @@
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -1069,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E75"/>
+  <dimension ref="A3:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1258,40 +1320,40 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="15"/>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
       <c r="D25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="15"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
@@ -1326,30 +1388,30 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="18" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E30" s="15"/>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="18"/>
-      <c r="E31" s="15"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="20"/>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
@@ -1359,66 +1421,66 @@
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="15"/>
+      <c r="E34" s="18"/>
     </row>
     <row r="35" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A35" s="17"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A36" s="17"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A37" s="17"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E37" s="15"/>
+      <c r="E37" s="18"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="E38" s="15"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
       <c r="D39" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="15"/>
+      <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
@@ -1436,18 +1498,18 @@
     </row>
     <row r="43" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="15"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="9" t="s">
         <v>84</v>
       </c>
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="B44" s="18"/>
-      <c r="C44" s="15"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="9" t="s">
         <v>85</v>
       </c>
@@ -1472,8 +1534,8 @@
       <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="B48" s="15"/>
-      <c r="C48" s="18" t="s">
+      <c r="B48" s="18"/>
+      <c r="C48" s="20" t="s">
         <v>88</v>
       </c>
       <c r="D48" s="9" t="s">
@@ -1481,15 +1543,15 @@
       </c>
     </row>
     <row r="49" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B49" s="15"/>
-      <c r="C49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="20"/>
       <c r="D49" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B50" s="15"/>
-      <c r="C50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="9" t="s">
         <v>91</v>
       </c>
@@ -1500,8 +1562,8 @@
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B52" s="15"/>
-      <c r="C52" s="18" t="s">
+      <c r="B52" s="18"/>
+      <c r="C52" s="20" t="s">
         <v>92</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -1509,15 +1571,15 @@
       </c>
     </row>
     <row r="53" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B53" s="15"/>
-      <c r="C53" s="18"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="20"/>
       <c r="D53" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B54" s="15"/>
-      <c r="C54" s="18"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="20"/>
       <c r="D54" s="9" t="s">
         <v>95</v>
       </c>
@@ -1528,8 +1590,8 @@
       <c r="D55" s="5"/>
     </row>
     <row r="56" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B56" s="15"/>
-      <c r="C56" s="18" t="s">
+      <c r="B56" s="18"/>
+      <c r="C56" s="20" t="s">
         <v>96</v>
       </c>
       <c r="D56" s="9" t="s">
@@ -1537,8 +1599,8 @@
       </c>
     </row>
     <row r="57" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B57" s="15"/>
-      <c r="C57" s="18"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="20"/>
       <c r="D57" s="9" t="s">
         <v>98</v>
       </c>
@@ -1577,8 +1639,8 @@
       <c r="D62" s="5"/>
     </row>
     <row r="63" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B63" s="15"/>
-      <c r="C63" s="18" t="s">
+      <c r="B63" s="18"/>
+      <c r="C63" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D63" s="9" t="s">
@@ -1586,8 +1648,8 @@
       </c>
     </row>
     <row r="64" spans="2:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="B64" s="15"/>
-      <c r="C64" s="18"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="9" t="s">
         <v>105</v>
       </c>
@@ -1622,58 +1684,201 @@
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B70" s="15"/>
-      <c r="C70" s="15"/>
-      <c r="D70" s="20" t="s">
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="15" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="71" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B71" s="15"/>
-      <c r="C71" s="15"/>
-      <c r="D71" s="20" t="s">
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B72" s="15"/>
-      <c r="C72" s="15"/>
-      <c r="D72" s="20" t="s">
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="15" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="73" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B73" s="15"/>
-      <c r="C73" s="15"/>
-      <c r="D73" s="20" t="s">
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
     </row>
     <row r="75" spans="2:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="20" t="s">
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="15" t="s">
         <v>112</v>
       </c>
     </row>
+    <row r="79" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C79" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" s="13"/>
+    </row>
+    <row r="80" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C80" s="13"/>
+      <c r="D80" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C81" s="13"/>
+      <c r="D81" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C82" s="13"/>
+      <c r="D82" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C83" s="13"/>
+      <c r="D83" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C84" s="13"/>
+      <c r="D84" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C85" s="13"/>
+      <c r="D85" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C86" s="13"/>
+      <c r="D86" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C87" s="13"/>
+      <c r="D87" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C88" s="13"/>
+      <c r="D88" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C89" s="13"/>
+      <c r="D89" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C90" s="13"/>
+      <c r="D90" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+    </row>
+    <row r="93" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C93" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D93" s="13"/>
+    </row>
+    <row r="94" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C94" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C95" s="13"/>
+      <c r="D95" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C96" s="13"/>
+      <c r="D96" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C97" s="13"/>
+      <c r="D97" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C98" s="13"/>
+      <c r="D98" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+    </row>
+    <row r="102" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C102" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D102" s="13"/>
+    </row>
+    <row r="103" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C103" s="18"/>
+      <c r="D103" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C104" s="18"/>
+      <c r="D104" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="C105" s="18"/>
+      <c r="D105" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C70:C75"/>
-    <mergeCell ref="B70:B75"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B56:B57"/>
+  <mergeCells count="25">
+    <mergeCell ref="C103:C105"/>
     <mergeCell ref="E22:E25"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="B22:B25"/>
@@ -1686,6 +1891,18 @@
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C70:C75"/>
+    <mergeCell ref="B70:B75"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B43:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1713,22 +1930,22 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
       <c r="C2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -1739,22 +1956,22 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>

</xml_diff>